<commit_message>
final timesheet fpr uploading
</commit_message>
<xml_diff>
--- a/Document/TimeSheet.xlsx
+++ b/Document/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jan" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -1516,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2028,144 +2028,300 @@
       <c r="B21" s="2">
         <v>41321</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="C21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="2">
         <v>41322</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="C22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="13">
+        <v>1</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="2">
         <v>41323</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="12">
+        <v>2</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="2">
         <v>41324</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="12">
+        <v>1</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="2">
         <v>41325</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="13">
+        <v>2</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="2">
         <v>41326</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="2">
         <v>41327</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="C27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="13">
+        <v>1</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="2">
         <v>41328</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="C28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="12">
+        <v>1</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="2">
         <v>41329</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="C29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="2">
         <v>41330</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="13">
+        <v>1</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="2">
         <v>41331</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="C31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="13">
+        <v>1</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="2">
         <v>41332</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="C32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="12">
+        <v>2</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="2">
         <v>41333</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="C33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="13">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2185,7 +2341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -3079,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3412,12 +3568,24 @@
       <c r="B14" s="2">
         <v>41373</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="C14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1</v>
+      </c>
       <c r="K14" s="5" t="s">
         <v>20</v>
       </c>
@@ -3429,12 +3597,24 @@
       <c r="B15" s="2">
         <v>41374</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="C15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="K15" s="5" t="s">
         <v>22</v>
       </c>
@@ -3446,12 +3626,24 @@
       <c r="B16" s="2">
         <v>41375</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="C16" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1</v>
+      </c>
       <c r="K16" s="8" t="s">
         <v>24</v>
       </c>
@@ -3463,209 +3655,413 @@
       <c r="B17" s="2">
         <v>41376</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="C17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="2">
         <v>41377</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="C18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="13">
+        <v>2</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="12">
+        <v>2</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="2">
         <v>41378</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="C19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="2">
         <v>41379</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="13">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="2">
         <v>41380</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="C21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="2">
         <v>41381</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="C22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="13">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="2">
         <v>41382</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="12">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="2">
         <v>41383</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="2">
         <v>41384</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="12">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="2">
         <v>41385</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="13">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="2">
         <v>41386</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="C27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="12">
+        <v>2</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="2">
         <v>41387</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="C28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="13">
+        <v>2</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="2">
         <v>41388</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="C29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="2">
         <v>41389</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="12">
+        <v>1</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="2">
         <v>41390</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="C31" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="2">
         <v>41391</v>
       </c>
-      <c r="C32" s="13"/>
+      <c r="C32" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
+      <c r="G32" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="2">
         <v>41392</v>
       </c>
-      <c r="C33" s="13"/>
+      <c r="C33" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="D33" s="13"/>
-      <c r="E33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F33" s="12"/>
-      <c r="G33" s="13"/>
+      <c r="G33" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="2">
         <v>41393</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="D34" s="13"/>
-      <c r="E34" s="12"/>
+      <c r="E34" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F34" s="12"/>
-      <c r="G34" s="13"/>
+      <c r="G34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="2">
         <v>41394</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="D35" s="13"/>
-      <c r="E35" s="12"/>
+      <c r="E35" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F35" s="12"/>
-      <c r="G35" s="13"/>
+      <c r="G35" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="H35" s="13"/>
     </row>
   </sheetData>

</xml_diff>